<commit_message>
need to fix gpu
</commit_message>
<xml_diff>
--- a/Output/Classifier Fitting/ResNet/label_mapping.xlsx
+++ b/Output/Classifier Fitting/ResNet/label_mapping.xlsx
@@ -458,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Convertible</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -468,7 +468,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Convertible</t>
+          <t>Pickup</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -478,7 +478,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>SUV</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>